<commit_message>
added updates and materials for capstone
</commit_message>
<xml_diff>
--- a/SantosAnea_CapstoneUpdates.xlsx
+++ b/SantosAnea_CapstoneUpdates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Capstone Project Title:</t>
   </si>
@@ -117,9 +117,6 @@
     </r>
   </si>
   <si>
-    <t>Mr. Jovi Gonzales</t>
-  </si>
-  <si>
     <t>Comments, Suggestions</t>
   </si>
   <si>
@@ -130,6 +127,36 @@
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>Include 'general public' as audience</t>
+  </si>
+  <si>
+    <t>Mr. Dizon</t>
+  </si>
+  <si>
+    <t>Mr. Gonzales</t>
+  </si>
+  <si>
+    <t>If it's aimed at children, consider adding a game</t>
+  </si>
+  <si>
+    <t>adviser should be able to help you to determine which information to include in the website</t>
+  </si>
+  <si>
+    <t>look for similar capstone projects to use as references</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>don't stop at 'awareness', 'educate' the viewers</t>
+  </si>
+  <si>
+    <t>use flash for game</t>
+  </si>
+  <si>
+    <t>group the volcanoes together (ex. List the active volcanoes in Luzon, Visayas, Mindanao)</t>
   </si>
 </sst>
 </file>
@@ -161,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -184,11 +211,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -204,6 +268,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,16 +581,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="93.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -535,29 +617,106 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+    </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="C9" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45">
+      <c r="A10" s="9"/>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30">
+      <c r="A11" s="9"/>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30">
+      <c r="A13" s="10"/>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A8:A13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>